<commit_message>
2001 Arrests clean up
</commit_message>
<xml_diff>
--- a/ope.ed.gov/2001/arrests-local-state-police-virginia-colleges-and-universities-crime-2001.xlsx
+++ b/ope.ed.gov/2001/arrests-local-state-police-virginia-colleges-and-universities-crime-2001.xlsx
@@ -13,16 +13,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
-    <t>Arrests - Local &amp; State Police</t>
-  </si>
-  <si>
-    <t>Survey year</t>
-  </si>
-  <si>
-    <t>Unitid</t>
-  </si>
-  <si>
-    <t>Institution name</t>
+    <t>Survey Year</t>
+  </si>
+  <si>
+    <t>UnitID</t>
+  </si>
+  <si>
+    <t>Institution Name</t>
   </si>
   <si>
     <t>Campus ID</t>
@@ -34,13 +31,13 @@
     <t>Institution Size</t>
   </si>
   <si>
-    <t>Illegal weapons possession</t>
-  </si>
-  <si>
-    <t>Drug law violations</t>
-  </si>
-  <si>
-    <t>Liquor law violations</t>
+    <t>Illegal Weapons Possession</t>
+  </si>
+  <si>
+    <t>Drug Law Violations</t>
+  </si>
+  <si>
+    <t>Liquor Law Violations</t>
   </si>
   <si>
     <t>Bryant &amp; Stratton College-Richmond</t>
@@ -247,34 +244,58 @@
       <c t="s" s="1" r="A1">
         <v>0</v>
       </c>
+      <c t="s" s="1" r="B1">
+        <v>1</v>
+      </c>
+      <c t="s" s="1" r="C1">
+        <v>2</v>
+      </c>
+      <c t="s" s="1" r="D1">
+        <v>3</v>
+      </c>
+      <c t="s" s="1" r="E1">
+        <v>4</v>
+      </c>
+      <c t="s" s="1" r="F1">
+        <v>5</v>
+      </c>
+      <c t="s" s="1" r="G1">
+        <v>6</v>
+      </c>
+      <c t="s" s="1" r="H1">
+        <v>7</v>
+      </c>
+      <c t="s" s="1" r="I1">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
-      <c t="s" s="1" r="A2">
-        <v>1</v>
-      </c>
-      <c t="s" s="1" r="B2">
-        <v>2</v>
+      <c s="1" r="A2">
+        <v>2001.0</v>
+      </c>
+      <c s="1" r="B2">
+        <v>231828.0</v>
       </c>
       <c t="s" s="1" r="C2">
-        <v>3</v>
-      </c>
-      <c t="s" s="1" r="D2">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c s="1" r="D2">
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E2">
-        <v>5</v>
-      </c>
-      <c t="s" s="1" r="F2">
-        <v>6</v>
-      </c>
-      <c t="s" s="1" r="G2">
-        <v>7</v>
-      </c>
-      <c t="s" s="1" r="H2">
-        <v>8</v>
-      </c>
-      <c t="s" s="1" r="I2">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c s="1" r="F2">
+        <v>295.0</v>
+      </c>
+      <c s="1" r="G2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="I2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
@@ -282,19 +303,19 @@
         <v>2001.0</v>
       </c>
       <c s="1" r="B3">
-        <v>231828.0</v>
+        <v>231785.0</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c s="1" r="D3">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c s="1" r="F3">
-        <v>295.0</v>
+        <v>297.0</v>
       </c>
       <c s="1" r="G3">
         <v>0.0</v>
@@ -311,28 +332,28 @@
         <v>2001.0</v>
       </c>
       <c s="1" r="B4">
-        <v>231785.0</v>
+        <v>232186.0</v>
       </c>
       <c t="s" s="1" r="C4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c s="1" r="D4">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c s="1" r="F4">
-        <v>297.0</v>
+        <v>24897.0</v>
       </c>
       <c s="1" r="G4">
-        <v>0.0</v>
+        <v>13.0</v>
       </c>
       <c s="1" r="H4">
-        <v>0.0</v>
+        <v>48.0</v>
       </c>
       <c s="1" r="I4">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="5">
@@ -340,28 +361,28 @@
         <v>2001.0</v>
       </c>
       <c s="1" r="B5">
-        <v>232186.0</v>
+        <v>406495.0</v>
       </c>
       <c t="s" s="1" r="C5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c s="1" r="D5">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c s="1" r="F5">
-        <v>24897.0</v>
+        <v>133.0</v>
       </c>
       <c s="1" r="G5">
-        <v>13.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="H5">
-        <v>48.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="I5">
-        <v>35.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
@@ -369,19 +390,19 @@
         <v>2001.0</v>
       </c>
       <c s="1" r="B6">
-        <v>406495.0</v>
+        <v>232557.0</v>
       </c>
       <c t="s" s="1" r="C6">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c s="1" r="D6">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E6">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c s="1" r="F6">
-        <v>133.0</v>
+        <v>6162.0</v>
       </c>
       <c s="1" r="G6">
         <v>0.0</v>
@@ -398,19 +419,19 @@
         <v>2001.0</v>
       </c>
       <c s="1" r="B7">
-        <v>232557.0</v>
+        <v>433299.0</v>
       </c>
       <c t="s" s="1" r="C7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c s="1" r="D7">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c s="1" r="F7">
-        <v>6162.0</v>
+        <v>34.0</v>
       </c>
       <c s="1" r="G7">
         <v>0.0</v>
@@ -427,19 +448,19 @@
         <v>2001.0</v>
       </c>
       <c s="1" r="B8">
-        <v>433299.0</v>
+        <v>233417.0</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c s="1" r="D8">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c s="1" r="F8">
-        <v>34.0</v>
+        <v>15.0</v>
       </c>
       <c s="1" r="G8">
         <v>0.0</v>
@@ -456,19 +477,19 @@
         <v>2001.0</v>
       </c>
       <c s="1" r="B9">
-        <v>233417.0</v>
+        <v>233310.0</v>
       </c>
       <c t="s" s="1" r="C9">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c s="1" r="D9">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E9">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c s="1" r="F9">
-        <v>15.0</v>
+        <v>2058.0</v>
       </c>
       <c s="1" r="G9">
         <v>0.0</v>
@@ -485,19 +506,19 @@
         <v>2001.0</v>
       </c>
       <c s="1" r="B10">
-        <v>233310.0</v>
+        <v>233338.0</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c s="1" r="D10">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E10">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c s="1" r="F10">
-        <v>2058.0</v>
+        <v>1304.0</v>
       </c>
       <c s="1" r="G10">
         <v>0.0</v>
@@ -514,19 +535,19 @@
         <v>2001.0</v>
       </c>
       <c s="1" r="B11">
-        <v>233338.0</v>
+        <v>233408.0</v>
       </c>
       <c t="s" s="1" r="C11">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c s="1" r="D11">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E11">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c s="1" r="F11">
-        <v>1304.0</v>
+        <v>136.0</v>
       </c>
       <c s="1" r="G11">
         <v>0.0</v>
@@ -543,19 +564,19 @@
         <v>2001.0</v>
       </c>
       <c s="1" r="B12">
-        <v>233408.0</v>
+        <v>233666.0</v>
       </c>
       <c t="s" s="1" r="C12">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c s="1" r="D12">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E12">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c s="1" r="F12">
-        <v>136.0</v>
+        <v>25.0</v>
       </c>
       <c s="1" r="G12">
         <v>0.0</v>
@@ -572,19 +593,19 @@
         <v>2001.0</v>
       </c>
       <c s="1" r="B13">
-        <v>233666.0</v>
+        <v>438498.0</v>
       </c>
       <c t="s" s="1" r="C13">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c s="1" r="D13">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E13">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c s="1" r="F13">
-        <v>25.0</v>
+        <v>686.0</v>
       </c>
       <c s="1" r="G13">
         <v>0.0</v>
@@ -601,19 +622,19 @@
         <v>2001.0</v>
       </c>
       <c s="1" r="B14">
-        <v>438498.0</v>
+        <v>233897.0</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c s="1" r="D14">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E14">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c s="1" r="F14">
-        <v>686.0</v>
+        <v>1480.0</v>
       </c>
       <c s="1" r="G14">
         <v>0.0</v>
@@ -630,19 +651,19 @@
         <v>2001.0</v>
       </c>
       <c s="1" r="B15">
-        <v>233897.0</v>
+        <v>234076.0</v>
       </c>
       <c t="s" s="1" r="C15">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c s="1" r="D15">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c t="s" s="1" r="E15">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c s="1" r="F15">
-        <v>1480.0</v>
+        <v>22739.0</v>
       </c>
       <c s="1" r="G15">
         <v>0.0</v>
@@ -662,19 +683,19 @@
         <v>234076.0</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c s="1" r="D16">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c t="s" s="1" r="E16">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c s="1" r="F16">
         <v>22739.0</v>
       </c>
       <c s="1" r="G16">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="H16">
         <v>0.0</v>
@@ -691,22 +712,22 @@
         <v>234076.0</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c s="1" r="D17">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c t="s" s="1" r="E17">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c s="1" r="F17">
         <v>22739.0</v>
       </c>
       <c s="1" r="G17">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="H17">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="I17">
         <v>0.0</v>
@@ -720,13 +741,13 @@
         <v>234076.0</v>
       </c>
       <c t="s" s="1" r="C18">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c s="1" r="D18">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c t="s" s="1" r="E18">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c s="1" r="F18">
         <v>22739.0</v>
@@ -735,7 +756,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="H18">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="I18">
         <v>0.0</v>
@@ -746,25 +767,25 @@
         <v>2001.0</v>
       </c>
       <c s="1" r="B19">
-        <v>234076.0</v>
+        <v>234030.0</v>
       </c>
       <c t="s" s="1" r="C19">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c s="1" r="D19">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E19">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c s="1" r="F19">
-        <v>22739.0</v>
+        <v>25001.0</v>
       </c>
       <c s="1" r="G19">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c s="1" r="H19">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c s="1" r="I19">
         <v>0.0</v>
@@ -778,13 +799,13 @@
         <v>234030.0</v>
       </c>
       <c t="s" s="1" r="C20">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c s="1" r="D20">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c t="s" s="1" r="E20">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c s="1" r="F20">
         <v>25001.0</v>
@@ -793,7 +814,7 @@
         <v>10.0</v>
       </c>
       <c s="1" r="H20">
-        <v>7.0</v>
+        <v>41.0</v>
       </c>
       <c s="1" r="I20">
         <v>0.0</v>
@@ -804,25 +825,25 @@
         <v>2001.0</v>
       </c>
       <c s="1" r="B21">
-        <v>234030.0</v>
+        <v>234119.0</v>
       </c>
       <c t="s" s="1" r="C21">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c s="1" r="D21">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E21">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c s="1" r="F21">
-        <v>25001.0</v>
+        <v>151.0</v>
       </c>
       <c s="1" r="G21">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="H21">
-        <v>41.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="I21">
         <v>0.0</v>
@@ -833,19 +854,19 @@
         <v>2001.0</v>
       </c>
       <c s="1" r="B22">
-        <v>234119.0</v>
+        <v>233949.0</v>
       </c>
       <c t="s" s="1" r="C22">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c s="1" r="D22">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E22">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c s="1" r="F22">
-        <v>151.0</v>
+        <v>7904.0</v>
       </c>
       <c s="1" r="G22">
         <v>0.0</v>
@@ -862,19 +883,19 @@
         <v>2001.0</v>
       </c>
       <c s="1" r="B23">
-        <v>233949.0</v>
+        <v>234191.0</v>
       </c>
       <c t="s" s="1" r="C23">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c s="1" r="D23">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E23">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c s="1" r="F23">
-        <v>7904.0</v>
+        <v>62.0</v>
       </c>
       <c s="1" r="G23">
         <v>0.0</v>
@@ -891,19 +912,19 @@
         <v>2001.0</v>
       </c>
       <c s="1" r="B24">
-        <v>234191.0</v>
+        <v>234359.0</v>
       </c>
       <c t="s" s="1" r="C24">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c s="1" r="D24">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E24">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c s="1" r="F24">
-        <v>62.0</v>
+        <v>238.0</v>
       </c>
       <c s="1" r="G24">
         <v>0.0</v>
@@ -912,35 +933,6 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I24">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c s="1" r="A25">
-        <v>2001.0</v>
-      </c>
-      <c s="1" r="B25">
-        <v>234359.0</v>
-      </c>
-      <c t="s" s="1" r="C25">
-        <v>54</v>
-      </c>
-      <c s="1" r="D25">
-        <v>1.0</v>
-      </c>
-      <c t="s" s="1" r="E25">
-        <v>55</v>
-      </c>
-      <c s="1" r="F25">
-        <v>238.0</v>
-      </c>
-      <c s="1" r="G25">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H25">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="I25">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>